<commit_message>
edit information in dataForGres (deleted gres calculations) and created script that annualizes emissions and graphs observed vs. G-res predicted emissions
</commit_message>
<xml_diff>
--- a/inputData/dataSources/dataForGres.xlsx
+++ b/inputData/dataSources/dataForGres.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\AA.AD.EPA.GOV\ORD\CIN\USERS\MAIN\F-K\JBEAULIE\Net MyDocuments\Documents\research\EPA\regionalOffices\region4\seminarData\inputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esilve02\RProjects\gRes\inputData\dataSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7335"/>
   </bookViews>
   <sheets>
     <sheet name="dataForGres" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="50">
   <si>
     <t>Lake_Name</t>
   </si>
@@ -48,24 +48,6 @@
     <t>ch4.trate.mg.h_Estimate</t>
   </si>
   <si>
-    <t>t.ch4.gCO2eq.m2.yr.gres</t>
-  </si>
-  <si>
-    <t>d.ch4.gCO2eq.m2.yr.gres</t>
-  </si>
-  <si>
-    <t>e.ch4.gCO2eq.m2.yr.gres</t>
-  </si>
-  <si>
-    <t>t.ch4.mgCH4.m2.hr.gres</t>
-  </si>
-  <si>
-    <t>d.ch4.mgCH4.m2.hr.gres</t>
-  </si>
-  <si>
-    <t>e.ch4.mgCH4.m2.hr.gres</t>
-  </si>
-  <si>
     <t>Acton Lake</t>
   </si>
   <si>
@@ -178,15 +160,6 @@
   </si>
   <si>
     <t>Watts Bar</t>
-  </si>
-  <si>
-    <t>ch4.drate.mg.m2.h_Estimate_Annual</t>
-  </si>
-  <si>
-    <t>ch4.erate.mg.h_Estimate_Annual</t>
-  </si>
-  <si>
-    <t>ch4.trate.mg.h_Estimate_Annual</t>
   </si>
   <si>
     <t>Survey</t>
@@ -1037,11 +1010,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,12 +1037,12 @@
     <col min="18" max="19" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1095,40 +1068,13 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N1" t="s">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C2">
         <v>2.2460837900000001</v>
@@ -1154,43 +1100,13 @@
       <c r="J2">
         <v>5.0875248500000003</v>
       </c>
-      <c r="K2">
-        <f>H2*0.25</f>
-        <v>0.42477228825000002</v>
-      </c>
-      <c r="L2">
-        <f t="shared" ref="L2:M2" si="0">I2*0.25</f>
-        <v>0.875427077</v>
-      </c>
-      <c r="M2">
-        <f t="shared" si="0"/>
-        <v>1.2718812125000001</v>
-      </c>
-      <c r="N2">
-        <v>208</v>
-      </c>
-      <c r="O2">
-        <v>145.6</v>
-      </c>
-      <c r="P2">
-        <v>62.4</v>
-      </c>
-      <c r="Q2">
-        <v>0.69836153599999995</v>
-      </c>
-      <c r="R2">
-        <v>0.48885307500000003</v>
-      </c>
-      <c r="S2">
-        <v>0.20950846100000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C3">
         <v>13.137</v>
@@ -1216,48 +1132,13 @@
       <c r="J3">
         <v>1.4427835600000001</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K33" si="1">H3*0.25</f>
-        <v>0.32145630325000002</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L33" si="2">I3*0.25</f>
-        <v>3.923958675E-2</v>
-      </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M33" si="3">J3*0.25</f>
-        <v>0.36069589000000002</v>
-      </c>
-      <c r="N3">
-        <v>73</v>
-      </c>
-      <c r="O3">
-        <f>N3*0.8</f>
-        <v>58.400000000000006</v>
-      </c>
-      <c r="P3">
-        <f>N3*0.2</f>
-        <v>14.600000000000001</v>
-      </c>
-      <c r="Q3">
-        <f t="shared" ref="Q3:S6" si="4">(N3*1000)/(365*24*34)</f>
-        <v>0.24509803921568626</v>
-      </c>
-      <c r="R3">
-        <f t="shared" si="4"/>
-        <v>0.19607843137254904</v>
-      </c>
-      <c r="S3">
-        <f t="shared" si="4"/>
-        <v>4.9019607843137261E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C4">
         <v>1.96277331</v>
@@ -1283,48 +1164,13 @@
       <c r="J4">
         <v>5.2537781140000002</v>
       </c>
-      <c r="K4">
-        <f t="shared" si="1"/>
-        <v>0.47285080725</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="2"/>
-        <v>0.84059372124999998</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="3"/>
-        <v>1.3134445285</v>
-      </c>
-      <c r="N4">
-        <v>186</v>
-      </c>
-      <c r="O4">
-        <f>N4*0.71</f>
-        <v>132.06</v>
-      </c>
-      <c r="P4">
-        <f>N4*0.29</f>
-        <v>53.94</v>
-      </c>
-      <c r="Q4">
-        <f t="shared" si="4"/>
-        <v>0.62449637389202262</v>
-      </c>
-      <c r="R4">
-        <f t="shared" si="4"/>
-        <v>0.44339242546333602</v>
-      </c>
-      <c r="S4">
-        <f t="shared" si="4"/>
-        <v>0.18110394842868655</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1">
         <v>6.0392540400000003</v>
@@ -1350,48 +1196,14 @@
       <c r="J5" s="1">
         <v>1.329108521</v>
       </c>
-      <c r="K5">
-        <f t="shared" si="1"/>
-        <v>0.23624396349999999</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="2"/>
-        <v>9.6033166749999996E-2</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="3"/>
-        <v>0.33227713025</v>
-      </c>
-      <c r="N5" s="1">
-        <v>217</v>
-      </c>
-      <c r="O5">
-        <f>N5*0.69</f>
-        <v>149.72999999999999</v>
-      </c>
-      <c r="P5">
-        <f>N5*0.31</f>
-        <v>67.27</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" si="4"/>
-        <v>0.72857910287402627</v>
-      </c>
-      <c r="R5">
-        <f t="shared" si="4"/>
-        <v>0.50271958098307812</v>
-      </c>
-      <c r="S5">
-        <f t="shared" si="4"/>
-        <v>0.22585952189094816</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <v>21.429914369999999</v>
@@ -1417,48 +1229,14 @@
       <c r="J6" s="1">
         <v>5.6780616029999997</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="1"/>
-        <v>0.10480554274999999</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="2"/>
-        <v>1.3230470974999999</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="3"/>
-        <v>1.4195154007499999</v>
-      </c>
-      <c r="N6" s="1">
-        <v>12</v>
-      </c>
-      <c r="O6">
-        <f>N6*0.93</f>
-        <v>11.16</v>
-      </c>
-      <c r="P6">
-        <f>N6*0.07</f>
-        <v>0.84000000000000008</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="4"/>
-        <v>4.0290088638195005E-2</v>
-      </c>
-      <c r="R6">
-        <f t="shared" si="4"/>
-        <v>3.7469782433521351E-2</v>
-      </c>
-      <c r="S6">
-        <f t="shared" si="4"/>
-        <v>2.8203062046736507E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C7">
         <v>4.5037827999999998</v>
@@ -1484,48 +1262,14 @@
       <c r="J7" s="1">
         <v>18.42922012</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="1"/>
-        <v>0.43413921875</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="2"/>
-        <v>4.2261096199999999</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="3"/>
-        <v>4.60730503</v>
-      </c>
-      <c r="N7" s="1">
-        <v>56</v>
-      </c>
-      <c r="O7">
-        <f>N7*0.83</f>
-        <v>46.48</v>
-      </c>
-      <c r="P7">
-        <f>N7*0.17</f>
-        <v>9.5200000000000014</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" ref="Q7:Q33" si="5">(N7*1000)/(365*24*34)</f>
-        <v>0.18802041364491001</v>
-      </c>
-      <c r="R7">
-        <f t="shared" ref="R7:R33" si="6">(O7*1000)/(365*24*34)</f>
-        <v>0.15605694332527531</v>
-      </c>
-      <c r="S7">
-        <f t="shared" ref="S7:S33" si="7">(P7*1000)/(365*24*34)</f>
-        <v>3.1963470319634708E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C8">
         <v>2.3448849200000002</v>
@@ -1551,48 +1295,14 @@
       <c r="J8" s="1">
         <v>2.8008334939999999</v>
       </c>
-      <c r="K8">
-        <f t="shared" si="1"/>
-        <v>0.58392141524999996</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="2"/>
-        <v>0.11628695825</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="3"/>
-        <v>0.70020837349999998</v>
-      </c>
-      <c r="N8" s="1">
-        <v>186</v>
-      </c>
-      <c r="O8">
-        <f>N8*0.71</f>
-        <v>132.06</v>
-      </c>
-      <c r="P8">
-        <f>N8*0.29</f>
-        <v>53.94</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="5"/>
-        <v>0.62449637389202262</v>
-      </c>
-      <c r="R8">
-        <f t="shared" si="6"/>
-        <v>0.44339242546333602</v>
-      </c>
-      <c r="S8">
-        <f t="shared" si="7"/>
-        <v>0.18110394842868655</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C9">
         <v>11.00550645</v>
@@ -1618,48 +1328,14 @@
       <c r="J9">
         <v>4.4740954339999996</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="1"/>
-        <v>0.66044097724999995</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="2"/>
-        <v>0.42382431225</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="3"/>
-        <v>1.1185238584999999</v>
-      </c>
-      <c r="N9" s="1">
-        <v>19</v>
-      </c>
-      <c r="O9">
-        <f>N9*0.9</f>
-        <v>17.100000000000001</v>
-      </c>
-      <c r="P9">
-        <f>N9*0.1</f>
-        <v>1.9000000000000001</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="5"/>
-        <v>6.3792640343808757E-2</v>
-      </c>
-      <c r="R9">
-        <f t="shared" si="6"/>
-        <v>5.7413376309427881E-2</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="7"/>
-        <v>6.3792640343808766E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C10">
         <v>2.14396904</v>
@@ -1685,48 +1361,14 @@
       <c r="J10">
         <v>0.87938522100000005</v>
       </c>
-      <c r="K10">
-        <f t="shared" si="1"/>
-        <v>0.20365360399999999</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="2"/>
-        <v>2.3988054500000001E-2</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="3"/>
-        <v>0.21984630525000001</v>
-      </c>
-      <c r="N10" s="1">
-        <v>101</v>
-      </c>
-      <c r="O10">
-        <f>N10*0.77</f>
-        <v>77.77</v>
-      </c>
-      <c r="P10">
-        <f>N10*0.23</f>
-        <v>23.23</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="5"/>
-        <v>0.33910824603814127</v>
-      </c>
-      <c r="R10">
-        <f t="shared" si="6"/>
-        <v>0.26111334944936881</v>
-      </c>
-      <c r="S10">
-        <f t="shared" si="7"/>
-        <v>7.7994896588772497E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C11">
         <v>32.208360540000001</v>
@@ -1752,48 +1394,14 @@
       <c r="J11">
         <v>4.0899004799999998</v>
       </c>
-      <c r="K11">
-        <f t="shared" si="1"/>
-        <v>0.30643383275000002</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="2"/>
-        <v>0.71392068075000004</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="3"/>
-        <v>1.02247512</v>
-      </c>
-      <c r="N11" s="1">
-        <v>121</v>
-      </c>
-      <c r="O11">
-        <f>N11*0.76</f>
-        <v>91.960000000000008</v>
-      </c>
-      <c r="P11">
-        <f>N11*0.24</f>
-        <v>29.04</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="5"/>
-        <v>0.40625839376846629</v>
-      </c>
-      <c r="R11">
-        <f t="shared" si="6"/>
-        <v>0.30875637926403443</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="7"/>
-        <v>9.7502014504431911E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C12">
         <v>4.8174293600000002</v>
@@ -1819,48 +1427,14 @@
       <c r="J12">
         <v>4.2237941399999999</v>
       </c>
-      <c r="K12">
-        <f t="shared" si="1"/>
-        <v>0.48454533950000001</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="2"/>
-        <v>0.60518413424999995</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="3"/>
-        <v>1.055948535</v>
-      </c>
-      <c r="N12" s="1">
-        <v>449</v>
-      </c>
-      <c r="O12">
-        <f>N12*0.6</f>
-        <v>269.39999999999998</v>
-      </c>
-      <c r="P12">
-        <f>N12*0.4</f>
-        <v>179.60000000000002</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="5"/>
-        <v>1.5075208165457965</v>
-      </c>
-      <c r="R12">
-        <f t="shared" si="6"/>
-        <v>0.90451248992747779</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="7"/>
-        <v>0.60300832661831871</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C13">
         <v>2.29135292</v>
@@ -1886,48 +1460,14 @@
       <c r="J13">
         <v>0.66603357699999999</v>
       </c>
-      <c r="K13">
-        <f t="shared" si="1"/>
-        <v>0.15430150249999999</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="2"/>
-        <v>0.1127184725</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="3"/>
-        <v>0.16650839425</v>
-      </c>
-      <c r="N13" s="1">
-        <v>172</v>
-      </c>
-      <c r="O13">
-        <f>N13*0.72</f>
-        <v>123.83999999999999</v>
-      </c>
-      <c r="P13">
-        <f>N13*0.28</f>
-        <v>48.160000000000004</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="5"/>
-        <v>0.57749127048079507</v>
-      </c>
-      <c r="R13">
-        <f t="shared" si="6"/>
-        <v>0.41579371474617238</v>
-      </c>
-      <c r="S13">
-        <f t="shared" si="7"/>
-        <v>0.16169755573462263</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C14">
         <v>4.4743415200000003</v>
@@ -1953,48 +1493,14 @@
       <c r="J14">
         <v>4.7667387110000004</v>
       </c>
-      <c r="K14">
-        <f t="shared" si="1"/>
-        <v>0.3779969695</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="2"/>
-        <v>0.84787189725000001</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="3"/>
-        <v>1.1916846777500001</v>
-      </c>
-      <c r="N14" s="1">
-        <v>318</v>
-      </c>
-      <c r="O14">
-        <f>N14*0.65</f>
-        <v>206.70000000000002</v>
-      </c>
-      <c r="P14">
-        <f>N14*0.35</f>
-        <v>111.3</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="5"/>
-        <v>1.0676873489121677</v>
-      </c>
-      <c r="R14">
-        <f t="shared" si="6"/>
-        <v>0.69399677679290905</v>
-      </c>
-      <c r="S14">
-        <f t="shared" si="7"/>
-        <v>0.37369057211925866</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C15">
         <v>5.2895770000000004</v>
@@ -2020,48 +1526,14 @@
       <c r="J15">
         <v>15.0305395</v>
       </c>
-      <c r="K15">
-        <f t="shared" si="1"/>
-        <v>0.40627667299999998</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="2"/>
-        <v>3.4124163925</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="3"/>
-        <v>3.7576348749999999</v>
-      </c>
-      <c r="N15" s="1">
-        <v>302</v>
-      </c>
-      <c r="O15">
-        <f>N15*0.65</f>
-        <v>196.3</v>
-      </c>
-      <c r="P15">
-        <f>N15*0.35</f>
-        <v>105.69999999999999</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="5"/>
-        <v>1.0139672307279075</v>
-      </c>
-      <c r="R15">
-        <f t="shared" si="6"/>
-        <v>0.65907869997313995</v>
-      </c>
-      <c r="S15">
-        <f t="shared" si="7"/>
-        <v>0.35488853075476762</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C16">
         <v>1.0422289300000001</v>
@@ -2087,48 +1559,14 @@
       <c r="J16">
         <v>5.0543851269999998</v>
       </c>
-      <c r="K16">
-        <f t="shared" si="1"/>
-        <v>0.71189897349999998</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="2"/>
-        <v>0.55169730824999996</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="3"/>
-        <v>1.2635962817499999</v>
-      </c>
-      <c r="N16" s="1">
-        <v>290</v>
-      </c>
-      <c r="O16">
-        <f>N16*0.66</f>
-        <v>191.4</v>
-      </c>
-      <c r="P16">
-        <f>N16*0.34</f>
-        <v>98.600000000000009</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="5"/>
-        <v>0.97367714208971257</v>
-      </c>
-      <c r="R16">
-        <f t="shared" si="6"/>
-        <v>0.64262691377921033</v>
-      </c>
-      <c r="S16">
-        <f t="shared" si="7"/>
-        <v>0.33105022831050235</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C17">
         <v>1.48090374</v>
@@ -2154,48 +1592,14 @@
       <c r="J17">
         <v>15.2068268</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="1"/>
-        <v>1.079471992</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="2"/>
-        <v>2.9381291049999998</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="3"/>
-        <v>3.8017067</v>
-      </c>
-      <c r="N17" s="1">
-        <v>449</v>
-      </c>
-      <c r="O17">
-        <f>N17*0.6</f>
-        <v>269.39999999999998</v>
-      </c>
-      <c r="P17">
-        <f>N17*0.4</f>
-        <v>179.60000000000002</v>
-      </c>
-      <c r="Q17">
-        <f t="shared" si="5"/>
-        <v>1.5075208165457965</v>
-      </c>
-      <c r="R17">
-        <f t="shared" si="6"/>
-        <v>0.90451248992747779</v>
-      </c>
-      <c r="S17">
-        <f t="shared" si="7"/>
-        <v>0.60300832661831871</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C18">
         <v>1.4795025399999999</v>
@@ -2221,48 +1625,14 @@
       <c r="J18">
         <v>2.7032453869999999</v>
       </c>
-      <c r="K18">
-        <f t="shared" si="1"/>
-        <v>0.20608792975000001</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="2"/>
-        <v>0.47905002400000002</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="3"/>
-        <v>0.67581134674999999</v>
-      </c>
-      <c r="N18" s="1">
-        <v>366</v>
-      </c>
-      <c r="O18">
-        <f>N18*0.63</f>
-        <v>230.58</v>
-      </c>
-      <c r="P18">
-        <f>N18*0.37</f>
-        <v>135.41999999999999</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="5"/>
-        <v>1.2288477034649476</v>
-      </c>
-      <c r="R18">
-        <f t="shared" si="6"/>
-        <v>0.77417405318291699</v>
-      </c>
-      <c r="S18">
-        <f t="shared" si="7"/>
-        <v>0.45467365028203061</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C19">
         <v>5.7705471199999998</v>
@@ -2288,48 +1658,14 @@
       <c r="J19">
         <v>5.5845281660000001</v>
       </c>
-      <c r="K19">
-        <f t="shared" si="1"/>
-        <v>0.10096961325000001</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="2"/>
-        <v>1.3022068200000001</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="3"/>
-        <v>1.3961320415</v>
-      </c>
-      <c r="N19" s="1">
-        <v>238</v>
-      </c>
-      <c r="O19">
-        <f>N19*0.68</f>
-        <v>161.84</v>
-      </c>
-      <c r="P19">
-        <f>N19*0.32</f>
-        <v>76.16</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" si="5"/>
-        <v>0.79908675799086759</v>
-      </c>
-      <c r="R19">
-        <f t="shared" si="6"/>
-        <v>0.54337899543378998</v>
-      </c>
-      <c r="S19">
-        <f t="shared" si="7"/>
-        <v>0.25570776255707761</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C20">
         <v>2.8476437099999998</v>
@@ -2355,48 +1691,14 @@
       <c r="J20">
         <v>12.30711425</v>
       </c>
-      <c r="K20">
-        <f t="shared" si="1"/>
-        <v>2.8584551499999999E-2</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="2"/>
-        <v>3.0574263949999998</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="3"/>
-        <v>3.0767785624999999</v>
-      </c>
-      <c r="N20" s="1">
-        <v>456</v>
-      </c>
-      <c r="O20">
-        <f>N20*0.6</f>
-        <v>273.59999999999997</v>
-      </c>
-      <c r="P20">
-        <f>N20*0.4</f>
-        <v>182.4</v>
-      </c>
-      <c r="Q20">
-        <f t="shared" si="5"/>
-        <v>1.5310233682514101</v>
-      </c>
-      <c r="R20">
-        <f t="shared" si="6"/>
-        <v>0.91861402095084588</v>
-      </c>
-      <c r="S20">
-        <f t="shared" si="7"/>
-        <v>0.61240934730056407</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C21">
         <v>6.5983785900000003</v>
@@ -2422,48 +1724,14 @@
       <c r="J21">
         <v>4.1094692820000001</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="1"/>
-        <v>0.15867672175</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="2"/>
-        <v>0.86869059900000001</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="3"/>
-        <v>1.0273673205</v>
-      </c>
-      <c r="N21" s="1">
-        <v>217</v>
-      </c>
-      <c r="O21">
-        <f>N21*0.69</f>
-        <v>149.72999999999999</v>
-      </c>
-      <c r="P21">
-        <f>N21*0.71</f>
-        <v>154.07</v>
-      </c>
-      <c r="Q21">
-        <f t="shared" si="5"/>
-        <v>0.72857910287402627</v>
-      </c>
-      <c r="R21">
-        <f t="shared" si="6"/>
-        <v>0.50271958098307812</v>
-      </c>
-      <c r="S21">
-        <f t="shared" si="7"/>
-        <v>0.51729116304055867</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C22">
         <v>2.0211599900000001</v>
@@ -2489,48 +1757,14 @@
       <c r="J22">
         <v>4.7878249999999998</v>
       </c>
-      <c r="K22">
-        <f t="shared" si="1"/>
-        <v>0.42752142524999998</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="2"/>
-        <v>0.80745668825000005</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="3"/>
-        <v>1.1969562499999999</v>
-      </c>
-      <c r="N22" s="1">
-        <v>290</v>
-      </c>
-      <c r="O22">
-        <f>N22*0.66</f>
-        <v>191.4</v>
-      </c>
-      <c r="P22">
-        <f>N22*0.34</f>
-        <v>98.600000000000009</v>
-      </c>
-      <c r="Q22">
-        <f t="shared" si="5"/>
-        <v>0.97367714208971257</v>
-      </c>
-      <c r="R22">
-        <f t="shared" si="6"/>
-        <v>0.64262691377921033</v>
-      </c>
-      <c r="S22">
-        <f t="shared" si="7"/>
-        <v>0.33105022831050235</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C23">
         <v>1.78133231</v>
@@ -2556,48 +1790,14 @@
       <c r="J23">
         <v>5.0226346570000002</v>
       </c>
-      <c r="K23">
-        <f t="shared" si="1"/>
-        <v>0.52809493674999997</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="2"/>
-        <v>0.76992738724999998</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="3"/>
-        <v>1.2556586642500001</v>
-      </c>
-      <c r="N23" s="1">
-        <v>246</v>
-      </c>
-      <c r="O23">
-        <f>N23*0.68</f>
-        <v>167.28</v>
-      </c>
-      <c r="P23">
-        <f>N23*0.32</f>
-        <v>78.72</v>
-      </c>
-      <c r="Q23">
-        <f t="shared" si="5"/>
-        <v>0.82594681708299755</v>
-      </c>
-      <c r="R23">
-        <f t="shared" si="6"/>
-        <v>0.56164383561643838</v>
-      </c>
-      <c r="S23">
-        <f t="shared" si="7"/>
-        <v>0.26430298146655923</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C24">
         <v>1.11772603</v>
@@ -2623,48 +1823,14 @@
       <c r="J24">
         <v>2.750633026</v>
       </c>
-      <c r="K24">
-        <f t="shared" si="1"/>
-        <v>0.30711067250000001</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="2"/>
-        <v>0.38054758399999999</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="3"/>
-        <v>0.68765825650000001</v>
-      </c>
-      <c r="N24" s="1">
-        <v>302</v>
-      </c>
-      <c r="O24">
-        <f>N24*0.65</f>
-        <v>196.3</v>
-      </c>
-      <c r="P24">
-        <f>N24*0.35</f>
-        <v>105.69999999999999</v>
-      </c>
-      <c r="Q24">
-        <f t="shared" si="5"/>
-        <v>1.0139672307279075</v>
-      </c>
-      <c r="R24">
-        <f t="shared" si="6"/>
-        <v>0.65907869997313995</v>
-      </c>
-      <c r="S24">
-        <f t="shared" si="7"/>
-        <v>0.35488853075476762</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C25">
         <v>9.1608824999999996</v>
@@ -2690,48 +1856,14 @@
       <c r="J25">
         <v>2.4653061539999999</v>
       </c>
-      <c r="K25">
-        <f t="shared" si="1"/>
-        <v>0.22177953149999999</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="2"/>
-        <v>0.39454700700000001</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="3"/>
-        <v>0.61632653849999997</v>
-      </c>
-      <c r="N25" s="1">
-        <v>167</v>
-      </c>
-      <c r="O25">
-        <f>N25*0.72</f>
-        <v>120.24</v>
-      </c>
-      <c r="P25">
-        <f>N25*0.28</f>
-        <v>46.760000000000005</v>
-      </c>
-      <c r="Q25">
-        <f t="shared" si="5"/>
-        <v>0.56070373354821379</v>
-      </c>
-      <c r="R25">
-        <f t="shared" si="6"/>
-        <v>0.40370668815471394</v>
-      </c>
-      <c r="S25">
-        <f t="shared" si="7"/>
-        <v>0.1569970453934999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C26">
         <v>4.6623825500000002</v>
@@ -2757,48 +1889,14 @@
       <c r="J26">
         <v>24.570694209999999</v>
       </c>
-      <c r="K26">
-        <f t="shared" si="1"/>
-        <v>0.56109291049999999</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="2"/>
-        <v>5.6937992225</v>
-      </c>
-      <c r="M26">
-        <f t="shared" si="3"/>
-        <v>6.1426735524999998</v>
-      </c>
-      <c r="N26" s="1">
-        <v>238</v>
-      </c>
-      <c r="O26">
-        <f>N26*0.68</f>
-        <v>161.84</v>
-      </c>
-      <c r="P26">
-        <f>N26*0.32</f>
-        <v>76.16</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" si="5"/>
-        <v>0.79908675799086759</v>
-      </c>
-      <c r="R26">
-        <f t="shared" si="6"/>
-        <v>0.54337899543378998</v>
-      </c>
-      <c r="S26">
-        <f t="shared" si="7"/>
-        <v>0.25570776255707761</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C27">
         <v>8.6729854300000007</v>
@@ -2824,48 +1922,14 @@
       <c r="J27">
         <v>0.51093838999999996</v>
       </c>
-      <c r="K27">
-        <f t="shared" si="1"/>
-        <v>5.8747282749999997E-2</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="2"/>
-        <v>6.8987314750000001E-2</v>
-      </c>
-      <c r="M27">
-        <f t="shared" si="3"/>
-        <v>0.12773459749999999</v>
-      </c>
-      <c r="N27" s="1">
-        <v>234</v>
-      </c>
-      <c r="O27">
-        <f>N27*0.68</f>
-        <v>159.12</v>
-      </c>
-      <c r="P27">
-        <f>N27*0.32</f>
-        <v>74.88</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" si="5"/>
-        <v>0.78565672844480261</v>
-      </c>
-      <c r="R27">
-        <f t="shared" si="6"/>
-        <v>0.53424657534246578</v>
-      </c>
-      <c r="S27">
-        <f t="shared" si="7"/>
-        <v>0.25141015310233683</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N27" s="1"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C28">
         <v>2.8296488900000001</v>
@@ -2891,48 +1955,14 @@
       <c r="J28">
         <v>5.4914990899999996</v>
       </c>
-      <c r="K28">
-        <f t="shared" si="1"/>
-        <v>0.37295339775000003</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="2"/>
-        <v>1.0438917700000001</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="3"/>
-        <v>1.3728747724999999</v>
-      </c>
-      <c r="N28" s="1">
-        <v>199</v>
-      </c>
-      <c r="O28">
-        <f>N28*0.7</f>
-        <v>139.29999999999998</v>
-      </c>
-      <c r="P28">
-        <f>N28*0.3</f>
-        <v>59.699999999999996</v>
-      </c>
-      <c r="Q28">
-        <f t="shared" si="5"/>
-        <v>0.66814396991673386</v>
-      </c>
-      <c r="R28">
-        <f t="shared" si="6"/>
-        <v>0.46770077894171358</v>
-      </c>
-      <c r="S28">
-        <f t="shared" si="7"/>
-        <v>0.20044319097502011</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N28" s="1"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C29">
         <v>6.7585995800000003</v>
@@ -2958,48 +1988,14 @@
       <c r="J29">
         <v>3.1869626630000001</v>
       </c>
-      <c r="K29">
-        <f t="shared" si="1"/>
-        <v>0.23792359574999999</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="2"/>
-        <v>0.58165421475000001</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="3"/>
-        <v>0.79674066575000002</v>
-      </c>
-      <c r="N29" s="1">
-        <v>149</v>
-      </c>
-      <c r="O29">
-        <f>N29*0.73</f>
-        <v>108.77</v>
-      </c>
-      <c r="P29">
-        <f>N29*0.27</f>
-        <v>40.230000000000004</v>
-      </c>
-      <c r="Q29">
-        <f t="shared" si="5"/>
-        <v>0.50026860059092126</v>
-      </c>
-      <c r="R29">
-        <f t="shared" si="6"/>
-        <v>0.36519607843137253</v>
-      </c>
-      <c r="S29">
-        <f t="shared" si="7"/>
-        <v>0.13507252215954876</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N29" s="1"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C30">
         <v>12.42437735</v>
@@ -3025,48 +2021,14 @@
       <c r="J30">
         <v>3.393438051</v>
       </c>
-      <c r="K30">
-        <f t="shared" si="1"/>
-        <v>0.181886202</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="2"/>
-        <v>0.66647331075000005</v>
-      </c>
-      <c r="M30">
-        <f t="shared" si="3"/>
-        <v>0.84835951274999999</v>
-      </c>
-      <c r="N30" s="1">
-        <v>208</v>
-      </c>
-      <c r="O30">
-        <f>N30*0.7</f>
-        <v>145.6</v>
-      </c>
-      <c r="P30">
-        <f>N30*0.3</f>
-        <v>62.4</v>
-      </c>
-      <c r="Q30">
-        <f t="shared" si="5"/>
-        <v>0.69836153639538012</v>
-      </c>
-      <c r="R30">
-        <f t="shared" si="6"/>
-        <v>0.48885307547676604</v>
-      </c>
-      <c r="S30">
-        <f t="shared" si="7"/>
-        <v>0.20950846091861403</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N30" s="1"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C31">
         <v>8.9417563799999993</v>
@@ -3092,48 +2054,14 @@
       <c r="J31">
         <v>0.68712601900000003</v>
       </c>
-      <c r="K31">
-        <f t="shared" si="1"/>
-        <v>0.147926694</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="2"/>
-        <v>2.3854811E-2</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="3"/>
-        <v>0.17178150475000001</v>
-      </c>
-      <c r="N31" s="1">
-        <v>225</v>
-      </c>
-      <c r="O31">
-        <f>N31*0.69</f>
-        <v>155.25</v>
-      </c>
-      <c r="P31">
-        <f>N31*0.31</f>
-        <v>69.75</v>
-      </c>
-      <c r="Q31">
-        <f t="shared" si="5"/>
-        <v>0.75543916196615635</v>
-      </c>
-      <c r="R31">
-        <f t="shared" si="6"/>
-        <v>0.52125302175664789</v>
-      </c>
-      <c r="S31">
-        <f t="shared" si="7"/>
-        <v>0.23418614020950845</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N31" s="1"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C32">
         <v>8.3194439599999992</v>
@@ -3159,48 +2087,14 @@
       <c r="J32">
         <v>10.12568686</v>
       </c>
-      <c r="K32">
-        <f t="shared" si="1"/>
-        <v>0.13525916374999999</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="2"/>
-        <v>2.43970187125</v>
-      </c>
-      <c r="M32">
-        <f t="shared" si="3"/>
-        <v>2.531421715</v>
-      </c>
-      <c r="N32" s="1">
-        <v>119</v>
-      </c>
-      <c r="O32">
-        <f>N32*0.76</f>
-        <v>90.44</v>
-      </c>
-      <c r="P32">
-        <f>N32*0.24</f>
-        <v>28.56</v>
-      </c>
-      <c r="Q32">
-        <f t="shared" si="5"/>
-        <v>0.3995433789954338</v>
-      </c>
-      <c r="R32">
-        <f t="shared" si="6"/>
-        <v>0.30365296803652969</v>
-      </c>
-      <c r="S32">
-        <f t="shared" si="7"/>
-        <v>9.5890410958904104E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N32" s="1"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C33">
         <v>1.3378338999999999</v>
@@ -3226,48 +2120,14 @@
       <c r="J33">
         <v>17.680053709999999</v>
       </c>
-      <c r="K33">
-        <f t="shared" si="1"/>
-        <v>1.2381469734999999</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="2"/>
-        <v>3.5120389799999998</v>
-      </c>
-      <c r="M33">
-        <f t="shared" si="3"/>
-        <v>4.4200134274999998</v>
-      </c>
-      <c r="N33" s="1">
-        <v>406</v>
-      </c>
-      <c r="O33">
-        <f>N33*0.62</f>
-        <v>251.72</v>
-      </c>
-      <c r="P33">
-        <f>N33*0.39</f>
-        <v>158.34</v>
-      </c>
-      <c r="Q33">
-        <f t="shared" si="5"/>
-        <v>1.3631479989255977</v>
-      </c>
-      <c r="R33">
-        <f t="shared" si="6"/>
-        <v>0.84515175933387054</v>
-      </c>
-      <c r="S33">
-        <f t="shared" si="7"/>
-        <v>0.53162771958098309</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N33" s="1"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C34">
         <v>49</v>
@@ -3293,43 +2153,13 @@
       <c r="J34">
         <v>1.2287414969999999</v>
       </c>
-      <c r="K34">
-        <f t="shared" ref="K34:K39" si="8">H34*0.25</f>
-        <v>0.144132653</v>
-      </c>
-      <c r="L34">
-        <f t="shared" ref="L34:L39" si="9">I34*0.25</f>
-        <v>0.16305272100000001</v>
-      </c>
-      <c r="M34">
-        <f t="shared" ref="M34:M39" si="10">J34*0.25</f>
-        <v>0.30718537424999998</v>
-      </c>
-      <c r="N34">
-        <v>285</v>
-      </c>
-      <c r="O34">
-        <v>162.44999999999999</v>
-      </c>
-      <c r="P34">
-        <v>122.55</v>
-      </c>
-      <c r="Q34">
-        <v>0.95688960499999998</v>
-      </c>
-      <c r="R34">
-        <v>0.54542707499999998</v>
-      </c>
-      <c r="S34">
-        <v>0.41146252999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C35">
         <v>115</v>
@@ -3355,43 +2185,13 @@
       <c r="J35">
         <v>0.31666666700000001</v>
       </c>
-      <c r="K35">
-        <f t="shared" si="8"/>
-        <v>7.9166666750000003E-2</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="M35">
-        <f t="shared" si="10"/>
-        <v>7.9166666750000003E-2</v>
-      </c>
-      <c r="N35">
-        <v>238</v>
-      </c>
-      <c r="O35">
-        <v>140.41999999999999</v>
-      </c>
-      <c r="P35">
-        <v>97.58</v>
-      </c>
-      <c r="Q35">
-        <v>0.79908675799999995</v>
-      </c>
-      <c r="R35">
-        <v>0.471461187</v>
-      </c>
-      <c r="S35">
-        <v>0.327625571</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" t="s">
         <v>49</v>
-      </c>
-      <c r="B36" t="s">
-        <v>58</v>
       </c>
       <c r="C36">
         <v>43</v>
@@ -3417,43 +2217,13 @@
       <c r="J36">
         <v>0.24321705399999999</v>
       </c>
-      <c r="K36">
-        <f t="shared" si="8"/>
-        <v>6.0804263499999997E-2</v>
-      </c>
-      <c r="L36">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="M36">
-        <f t="shared" si="10"/>
-        <v>6.0804263499999997E-2</v>
-      </c>
-      <c r="N36">
-        <v>90</v>
-      </c>
-      <c r="O36">
-        <v>53.1</v>
-      </c>
-      <c r="P36">
-        <v>36.9</v>
-      </c>
-      <c r="Q36">
-        <v>0.30217566499999998</v>
-      </c>
-      <c r="R36">
-        <v>0.17828364199999999</v>
-      </c>
-      <c r="S36">
-        <v>0.123892023</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C37">
         <v>279</v>
@@ -3479,43 +2249,13 @@
       <c r="J37">
         <v>0.79584826799999997</v>
       </c>
-      <c r="K37">
-        <f t="shared" si="8"/>
-        <v>5.58169055E-2</v>
-      </c>
-      <c r="L37">
-        <f t="shared" si="9"/>
-        <v>0.14314516125000001</v>
-      </c>
-      <c r="M37">
-        <f t="shared" si="10"/>
-        <v>0.19896206699999999</v>
-      </c>
-      <c r="N37">
-        <v>456</v>
-      </c>
-      <c r="O37">
-        <v>269.04000000000002</v>
-      </c>
-      <c r="P37">
-        <v>186.96</v>
-      </c>
-      <c r="Q37">
-        <v>1.5310233680000001</v>
-      </c>
-      <c r="R37">
-        <v>0.90330378700000002</v>
-      </c>
-      <c r="S37">
-        <v>0.62771958100000003</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C38">
         <v>226</v>
@@ -3541,43 +2281,13 @@
       <c r="J38">
         <v>0.95833333300000001</v>
       </c>
-      <c r="K38">
-        <f t="shared" si="8"/>
-        <v>0.23741703550000001</v>
-      </c>
-      <c r="L38">
-        <f t="shared" si="9"/>
-        <v>2.1662980000000001E-3</v>
-      </c>
-      <c r="M38">
-        <f t="shared" si="10"/>
-        <v>0.23958333325</v>
-      </c>
-      <c r="N38">
-        <v>206</v>
-      </c>
-      <c r="O38">
-        <v>125.66</v>
-      </c>
-      <c r="P38">
-        <v>80.34</v>
-      </c>
-      <c r="Q38">
-        <v>0.69164652199999999</v>
-      </c>
-      <c r="R38">
-        <v>0.42190437800000002</v>
-      </c>
-      <c r="S38">
-        <v>0.26974214299999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C39">
         <v>176</v>
@@ -3602,36 +2312,6 @@
       </c>
       <c r="J39">
         <v>4.2807335000000002E-2</v>
-      </c>
-      <c r="K39">
-        <f t="shared" si="8"/>
-        <v>9.3298037500000007E-3</v>
-      </c>
-      <c r="L39">
-        <f t="shared" si="9"/>
-        <v>1.37203E-3</v>
-      </c>
-      <c r="M39">
-        <f t="shared" si="10"/>
-        <v>1.070183375E-2</v>
-      </c>
-      <c r="N39">
-        <v>276</v>
-      </c>
-      <c r="O39">
-        <v>157.32</v>
-      </c>
-      <c r="P39">
-        <v>118.68</v>
-      </c>
-      <c r="Q39">
-        <v>0.92667203899999995</v>
-      </c>
-      <c r="R39">
-        <v>0.528203062</v>
-      </c>
-      <c r="S39">
-        <v>0.398468977</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited annualizeEmissions R file and inputted more data into G-res (harrison and extra land use  data)
</commit_message>
<xml_diff>
--- a/inputData/dataSources/dataForGres.xlsx
+++ b/inputData/dataSources/dataForGres.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="53">
   <si>
     <t>Lake_Name</t>
   </si>
@@ -169,6 +169,15 @@
   </si>
   <si>
     <t>Bevelhimer</t>
+  </si>
+  <si>
+    <t>William H Harsha Lake 2017</t>
+  </si>
+  <si>
+    <t>William H Harsha Lake 2016</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -1010,11 +1019,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,6 +2323,166 @@
         <v>4.2807335000000002E-2</v>
       </c>
     </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40">
+        <v>8.3194439599999992</v>
+      </c>
+      <c r="D40">
+        <v>34.451219510000001</v>
+      </c>
+      <c r="E40">
+        <v>9.5912589000000006E-2</v>
+      </c>
+      <c r="F40">
+        <v>11.629</v>
+      </c>
+      <c r="G40">
+        <v>0.1552</v>
+      </c>
+      <c r="H40">
+        <v>2</v>
+      </c>
+      <c r="I40">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="J40">
+        <v>34.299999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41">
+        <v>8.3194439599999992</v>
+      </c>
+      <c r="D41">
+        <v>34.451219510000001</v>
+      </c>
+      <c r="E41">
+        <v>9.5912589000000006E-2</v>
+      </c>
+      <c r="F41">
+        <v>11.629</v>
+      </c>
+      <c r="G41">
+        <v>0.1552</v>
+      </c>
+      <c r="H41">
+        <v>0.6</v>
+      </c>
+      <c r="I41">
+        <v>7.7</v>
+      </c>
+      <c r="J41">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" t="s">
+        <v>52</v>
+      </c>
+      <c r="E42" t="s">
+        <v>52</v>
+      </c>
+      <c r="F42" t="s">
+        <v>52</v>
+      </c>
+      <c r="G42" t="s">
+        <v>52</v>
+      </c>
+      <c r="H42" t="s">
+        <v>52</v>
+      </c>
+      <c r="I42" t="s">
+        <v>52</v>
+      </c>
+      <c r="J42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" t="s">
+        <v>52</v>
+      </c>
+      <c r="F43" t="s">
+        <v>52</v>
+      </c>
+      <c r="G43" t="s">
+        <v>52</v>
+      </c>
+      <c r="H43" t="s">
+        <v>52</v>
+      </c>
+      <c r="I43" t="s">
+        <v>52</v>
+      </c>
+      <c r="J43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" t="s">
+        <v>52</v>
+      </c>
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="F44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44" t="s">
+        <v>52</v>
+      </c>
+      <c r="H44" t="s">
+        <v>52</v>
+      </c>
+      <c r="I44" t="s">
+        <v>52</v>
+      </c>
+      <c r="J44" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>